<commit_message>
transactions + division code + fix bug
</commit_message>
<xml_diff>
--- a/backend/users.xlsx
+++ b/backend/users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Utilisateurs" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -419,7 +419,7 @@
         <v>gear</v>
       </c>
       <c r="F1" t="str">
-        <v>refundBalance</v>
+        <v>transactions</v>
       </c>
     </row>
     <row r="2">
@@ -433,13 +433,13 @@
         <v>true</v>
       </c>
       <c r="D2" t="str">
-        <v>["jeudi","vendredi","samedi","dimanche"]</v>
+        <v>["jeudi","samedi","vendredi","dimanche"]</v>
       </c>
       <c r="E2" t="str">
-        <v>[{"item":"Jardin","quantity":1},{"item":"Matelas","quantity":4}]</v>
-      </c>
-      <c r="F2">
-        <v>-15</v>
+        <v>[{"item":"Jardin","quantity":8},{"item":"Matelas","quantity":4}]</v>
+      </c>
+      <c r="F2" t="str">
+        <v>[]</v>
       </c>
     </row>
     <row r="3">
@@ -449,8 +449,8 @@
       <c r="B3" t="str">
         <v>Ju</v>
       </c>
-      <c r="C3" t="str">
-        <v>false</v>
+      <c r="C3" t="b">
+        <v>0</v>
       </c>
       <c r="D3" t="str">
         <v>[]</v>
@@ -458,13 +458,33 @@
       <c r="E3" t="str">
         <v>[]</v>
       </c>
-      <c r="F3">
-        <v>0</v>
+      <c r="F3" t="str">
+        <v>[{"id":"1745428649532","payer":"Ju","amount":666,"description":"d","repayments":[{"userId":"Mila","amount":222,"paid":false},{"userId":"Ju","amount":222,"paid":false},{"userId":"Louise","amount":222,"paid":false}]}]</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>1745427357665</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Louise</v>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v>[]</v>
+      </c>
+      <c r="E4" t="str">
+        <v>[]</v>
+      </c>
+      <c r="F4" t="str">
+        <v>[]</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Debut HomePage : course + playlist + photos
</commit_message>
<xml_diff>
--- a/backend/users.xlsx
+++ b/backend/users.xlsx
@@ -439,7 +439,7 @@
         <v>[{"item":"Jardin","quantity":8},{"item":"Matelas","quantity":4}]</v>
       </c>
       <c r="F2" t="str">
-        <v>[]</v>
+        <v>[{"id":"1745434641049","payer":"Mila","amount":200,"description":"Courses","repayments":[{"userId":"Mila","amount":66.67,"paid":false},{"userId":"Ju","amount":66.67,"paid":false},{"userId":"Louise","amount":66.67,"paid":false}]}]</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         <v>[]</v>
       </c>
       <c r="F3" t="str">
-        <v>[{"id":"1745428649532","payer":"Ju","amount":666,"description":"d","repayments":[{"userId":"Mila","amount":222,"paid":false},{"userId":"Ju","amount":222,"paid":false},{"userId":"Louise","amount":222,"paid":false}]}]</v>
+        <v>[]</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
transactions bien peu faire mieux
</commit_message>
<xml_diff>
--- a/backend/users.xlsx
+++ b/backend/users.xlsx
@@ -433,13 +433,13 @@
         <v>true</v>
       </c>
       <c r="D2" t="str">
-        <v>["jeudi","samedi","vendredi","dimanche"]</v>
+        <v>["jeudi","samedi","dimanche"]</v>
       </c>
       <c r="E2" t="str">
         <v>[{"item":"Jardin","quantity":8},{"item":"Matelas","quantity":4}]</v>
       </c>
       <c r="F2" t="str">
-        <v>[{"id":"1745489437932","payer":"Mila","amount":300,"description":"Course","repayments":[{"userId":"Mila","amount":100,"paid":false},{"userId":"Ju","amount":100,"paid":false},{"userId":"Louise","amount":100,"paid":false}]},{"id":"1745489746144","payer":"Mila","amount":5562,"description":"ddd","repayments":[{"userId":"Mila","amount":1854,"paid":false},{"userId":"Ju","amount":1854,"paid":false},{"userId":"Louise","amount":1854,"paid":false}]}]</v>
+        <v>[{"transactionId":"1745665348518","payer":"Mila","amount":185,"description":"test","repayments":[{"userId":"Mila","amount":185,"paid":false}],"paid":false}]</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         <v>[{"item":"test","quantity":1}]</v>
       </c>
       <c r="F3" t="str">
-        <v>[]</v>
+        <v>[{"transactionId":"1745665348518","payer":"Mila","amount":185,"description":"test","repayments":[{"userId":"Ju","amount":185,"paid":false}],"paid":false}]</v>
       </c>
     </row>
     <row r="4">
@@ -479,7 +479,7 @@
         <v>[{"item":"blabla","quantity":1}]</v>
       </c>
       <c r="F4" t="str">
-        <v>[]</v>
+        <v>[{"transactionId":"1745665348518","payer":"Mila","amount":185,"description":"test","repayments":[{"userId":"Louise","amount":185,"paid":false}],"paid":false}]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>